<commit_message>
bye bye preview packages
</commit_message>
<xml_diff>
--- a/Data/Input/EmployeesInformations.xlsx
+++ b/Data/Input/EmployeesInformations.xlsx
@@ -1273,26 +1273,26 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D2" r:id="rId29"/>
-    <x:hyperlink ref="D3" r:id="rId30"/>
-    <x:hyperlink ref="D4" r:id="rId31"/>
-    <x:hyperlink ref="D5" r:id="rId32"/>
-    <x:hyperlink ref="D6" r:id="rId33"/>
-    <x:hyperlink ref="D7" r:id="rId34"/>
-    <x:hyperlink ref="D8" r:id="rId35"/>
-    <x:hyperlink ref="D9" r:id="rId36"/>
-    <x:hyperlink ref="D10" r:id="rId37"/>
-    <x:hyperlink ref="F10" r:id="rId38"/>
-    <x:hyperlink ref="F2" r:id="rId39"/>
-    <x:hyperlink ref="F3" r:id="rId40"/>
-    <x:hyperlink ref="F4" r:id="rId61"/>
-    <x:hyperlink ref="F6" r:id="rId62"/>
-    <x:hyperlink ref="F5" r:id="rId63"/>
-    <x:hyperlink ref="F7" r:id="rId64"/>
-    <x:hyperlink ref="F8" r:id="rId65"/>
-    <x:hyperlink ref="F9" r:id="rId66"/>
-    <x:hyperlink ref="D11" r:id="rId67"/>
-    <x:hyperlink ref="F11" r:id="rId68"/>
+    <x:hyperlink ref="D2" r:id="rId41"/>
+    <x:hyperlink ref="D3" r:id="rId42"/>
+    <x:hyperlink ref="D4" r:id="rId43"/>
+    <x:hyperlink ref="D5" r:id="rId44"/>
+    <x:hyperlink ref="D6" r:id="rId45"/>
+    <x:hyperlink ref="D7" r:id="rId46"/>
+    <x:hyperlink ref="D8" r:id="rId47"/>
+    <x:hyperlink ref="D9" r:id="rId48"/>
+    <x:hyperlink ref="D10" r:id="rId49"/>
+    <x:hyperlink ref="F10" r:id="rId50"/>
+    <x:hyperlink ref="F2" r:id="rId51"/>
+    <x:hyperlink ref="F3" r:id="rId52"/>
+    <x:hyperlink ref="F4" r:id="rId53"/>
+    <x:hyperlink ref="F6" r:id="rId54"/>
+    <x:hyperlink ref="F5" r:id="rId55"/>
+    <x:hyperlink ref="F7" r:id="rId56"/>
+    <x:hyperlink ref="F8" r:id="rId57"/>
+    <x:hyperlink ref="F9" r:id="rId58"/>
+    <x:hyperlink ref="D11" r:id="rId59"/>
+    <x:hyperlink ref="F11" r:id="rId60"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1393,10 +1393,10 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="C2" r:id="rId69"/>
-    <x:hyperlink ref="C3" r:id="rId70"/>
-    <x:hyperlink ref="C4" r:id="rId71"/>
-    <x:hyperlink ref="C5" r:id="rId72"/>
+    <x:hyperlink ref="C2" r:id="rId73"/>
+    <x:hyperlink ref="C3" r:id="rId74"/>
+    <x:hyperlink ref="C4" r:id="rId75"/>
+    <x:hyperlink ref="C5" r:id="rId76"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1668,19 +1668,19 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="C2" r:id="rId78"/>
-    <x:hyperlink ref="C3" r:id="rId79"/>
-    <x:hyperlink ref="C4" r:id="rId80"/>
-    <x:hyperlink ref="C5" r:id="rId81"/>
-    <x:hyperlink ref="C6" r:id="rId82"/>
-    <x:hyperlink ref="C7" r:id="rId83"/>
-    <x:hyperlink ref="C8" r:id="rId84"/>
-    <x:hyperlink ref="C9" r:id="rId85"/>
-    <x:hyperlink ref="C10" r:id="rId86"/>
-    <x:hyperlink ref="C11" r:id="rId87"/>
-    <x:hyperlink ref="C12" r:id="rId88"/>
-    <x:hyperlink ref="C13" r:id="rId89"/>
-    <x:hyperlink ref="C14" r:id="rId90"/>
+    <x:hyperlink ref="C2" r:id="rId77"/>
+    <x:hyperlink ref="C3" r:id="rId91"/>
+    <x:hyperlink ref="C4" r:id="rId92"/>
+    <x:hyperlink ref="C5" r:id="rId93"/>
+    <x:hyperlink ref="C6" r:id="rId94"/>
+    <x:hyperlink ref="C7" r:id="rId95"/>
+    <x:hyperlink ref="C8" r:id="rId96"/>
+    <x:hyperlink ref="C9" r:id="rId97"/>
+    <x:hyperlink ref="C10" r:id="rId98"/>
+    <x:hyperlink ref="C11" r:id="rId99"/>
+    <x:hyperlink ref="C12" r:id="rId100"/>
+    <x:hyperlink ref="C13" r:id="rId101"/>
+    <x:hyperlink ref="C14" r:id="rId102"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1749,10 +1749,10 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A2" r:id="rId91"/>
-    <x:hyperlink ref="A3" r:id="rId92"/>
-    <x:hyperlink ref="A4" r:id="rId93"/>
-    <x:hyperlink ref="A5" r:id="rId94"/>
+    <x:hyperlink ref="A2" r:id="rId103"/>
+    <x:hyperlink ref="A3" r:id="rId104"/>
+    <x:hyperlink ref="A4" r:id="rId105"/>
+    <x:hyperlink ref="A5" r:id="rId106"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished the GetFormResponses wf
</commit_message>
<xml_diff>
--- a/Data/Input/EmployeesInformations.xlsx
+++ b/Data/Input/EmployeesInformations.xlsx
@@ -5,19 +5,19 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate\RPA\MetaMarian\MetaMarian_Robot\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate\RPA\MetaMarian\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F30326-CF63-474B-A31A-1E6DC1925B38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5946485-AE37-4A11-97E2-4C9F786C00A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Employees" sheetId="1" r:id="rId1"/>
     <x:sheet name="Managers" sheetId="2" r:id="rId2"/>
     <x:sheet name="Mentors" sheetId="3" r:id="rId3"/>
     <x:sheet name="UsefulLinks" sheetId="4" r:id="rId4"/>
-    <x:sheet name="PracticeFormular" sheetId="5" r:id="rId5"/>
+    <x:sheet name="PracticeForm" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191028"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <x:si>
     <x:t>First Name</x:t>
   </x:si>
@@ -517,16 +517,127 @@
     <x:t>Introduction in JavaScript</x:t>
   </x:si>
   <x:si>
+    <x:t>Processed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Employee id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Field of study(specialization)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Group</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Year of studies</x:t>
+  </x:si>
+  <x:si>
     <x:t>Faculty</x:t>
   </x:si>
   <x:si>
     <x:t>University</x:t>
   </x:si>
   <x:si>
-    <x:t>Position in company</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Number of hours of practice</x:t>
+    <x:t>Number of practical hours required</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dada</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dsffsd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ff</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fafaf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>grge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vdffd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fefe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hfhf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jghj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hjk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>khk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kuh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>,nj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>khu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kjkgh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vfd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>da</x:t>
+  </x:si>
+  <x:si>
+    <x:t>address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>csd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vsdv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vsdd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hfg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>wwd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>czc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dwefwe</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -536,7 +647,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="4" x14ac:knownFonts="1">
+  <x:fonts count="5" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -558,6 +669,12 @@
       <x:name val="Calibri"/>
     </x:font>
     <x:font>
+      <x:sz val="10"/>
+      <x:color theme="1"/>
+      <x:name val="Arial"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -573,7 +690,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border>
       <x:left/>
       <x:right/>
@@ -581,8 +698,23 @@
       <x:bottom/>
       <x:diagonal/>
     </x:border>
+    <x:border>
+      <x:left style="medium">
+        <x:color rgb="FFCCCCCC"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color rgb="FFCCCCCC"/>
+      </x:right>
+      <x:top style="medium">
+        <x:color rgb="FFCCCCCC"/>
+      </x:top>
+      <x:bottom style="medium">
+        <x:color rgb="FFCCCCCC"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="4">
+  <x:cellStyleXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -591,14 +723,22 @@
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <x:alignment wrapText="1"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </x:cellXfs>
   <x:cellStyles count="2">
     <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1273,26 +1413,26 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D2" r:id="rId41"/>
-    <x:hyperlink ref="D3" r:id="rId42"/>
-    <x:hyperlink ref="D4" r:id="rId43"/>
-    <x:hyperlink ref="D5" r:id="rId44"/>
-    <x:hyperlink ref="D6" r:id="rId45"/>
-    <x:hyperlink ref="D7" r:id="rId46"/>
-    <x:hyperlink ref="D8" r:id="rId47"/>
-    <x:hyperlink ref="D9" r:id="rId48"/>
-    <x:hyperlink ref="D10" r:id="rId49"/>
-    <x:hyperlink ref="F10" r:id="rId50"/>
-    <x:hyperlink ref="F2" r:id="rId51"/>
-    <x:hyperlink ref="F3" r:id="rId52"/>
-    <x:hyperlink ref="F4" r:id="rId53"/>
-    <x:hyperlink ref="F6" r:id="rId54"/>
-    <x:hyperlink ref="F5" r:id="rId55"/>
-    <x:hyperlink ref="F7" r:id="rId56"/>
-    <x:hyperlink ref="F8" r:id="rId57"/>
-    <x:hyperlink ref="F9" r:id="rId58"/>
-    <x:hyperlink ref="D11" r:id="rId59"/>
-    <x:hyperlink ref="F11" r:id="rId60"/>
+    <x:hyperlink ref="D2" r:id="rId29"/>
+    <x:hyperlink ref="D3" r:id="rId30"/>
+    <x:hyperlink ref="D4" r:id="rId31"/>
+    <x:hyperlink ref="D5" r:id="rId32"/>
+    <x:hyperlink ref="D6" r:id="rId33"/>
+    <x:hyperlink ref="D7" r:id="rId34"/>
+    <x:hyperlink ref="D8" r:id="rId35"/>
+    <x:hyperlink ref="D9" r:id="rId36"/>
+    <x:hyperlink ref="D10" r:id="rId37"/>
+    <x:hyperlink ref="F10" r:id="rId38"/>
+    <x:hyperlink ref="F2" r:id="rId39"/>
+    <x:hyperlink ref="F3" r:id="rId40"/>
+    <x:hyperlink ref="F4" r:id="rId61"/>
+    <x:hyperlink ref="F6" r:id="rId62"/>
+    <x:hyperlink ref="F5" r:id="rId63"/>
+    <x:hyperlink ref="F7" r:id="rId64"/>
+    <x:hyperlink ref="F8" r:id="rId65"/>
+    <x:hyperlink ref="F9" r:id="rId66"/>
+    <x:hyperlink ref="D11" r:id="rId67"/>
+    <x:hyperlink ref="F11" r:id="rId68"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1393,10 +1533,10 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="C2" r:id="rId73"/>
-    <x:hyperlink ref="C3" r:id="rId74"/>
-    <x:hyperlink ref="C4" r:id="rId75"/>
-    <x:hyperlink ref="C5" r:id="rId76"/>
+    <x:hyperlink ref="C2" r:id="rId69"/>
+    <x:hyperlink ref="C3" r:id="rId70"/>
+    <x:hyperlink ref="C4" r:id="rId71"/>
+    <x:hyperlink ref="C5" r:id="rId72"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,7 +1553,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:E14"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="G15" sqref="G15"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1668,19 +1808,19 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="C2" r:id="rId77"/>
-    <x:hyperlink ref="C3" r:id="rId91"/>
-    <x:hyperlink ref="C4" r:id="rId92"/>
-    <x:hyperlink ref="C5" r:id="rId93"/>
-    <x:hyperlink ref="C6" r:id="rId94"/>
-    <x:hyperlink ref="C7" r:id="rId95"/>
-    <x:hyperlink ref="C8" r:id="rId96"/>
-    <x:hyperlink ref="C9" r:id="rId97"/>
-    <x:hyperlink ref="C10" r:id="rId98"/>
-    <x:hyperlink ref="C11" r:id="rId99"/>
-    <x:hyperlink ref="C12" r:id="rId100"/>
-    <x:hyperlink ref="C13" r:id="rId101"/>
-    <x:hyperlink ref="C14" r:id="rId102"/>
+    <x:hyperlink ref="C2" r:id="rId78"/>
+    <x:hyperlink ref="C3" r:id="rId79"/>
+    <x:hyperlink ref="C4" r:id="rId80"/>
+    <x:hyperlink ref="C5" r:id="rId81"/>
+    <x:hyperlink ref="C6" r:id="rId82"/>
+    <x:hyperlink ref="C7" r:id="rId83"/>
+    <x:hyperlink ref="C8" r:id="rId84"/>
+    <x:hyperlink ref="C9" r:id="rId85"/>
+    <x:hyperlink ref="C10" r:id="rId86"/>
+    <x:hyperlink ref="C11" r:id="rId87"/>
+    <x:hyperlink ref="C12" r:id="rId88"/>
+    <x:hyperlink ref="C13" r:id="rId89"/>
+    <x:hyperlink ref="C14" r:id="rId90"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1749,10 +1889,10 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A2" r:id="rId103"/>
-    <x:hyperlink ref="A3" r:id="rId104"/>
-    <x:hyperlink ref="A4" r:id="rId105"/>
-    <x:hyperlink ref="A5" r:id="rId106"/>
+    <x:hyperlink ref="A2" r:id="rId107"/>
+    <x:hyperlink ref="A3" r:id="rId108"/>
+    <x:hyperlink ref="A4" r:id="rId109"/>
+    <x:hyperlink ref="A5" r:id="rId110"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1767,50 +1907,194 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G1"/>
+  <x:dimension ref="A1:N1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="F7" sqref="F7"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C6" sqref="C6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
-    <x:col min="1" max="1" width="19.179688" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="17.269531" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="15.542969" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="17" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="16.269531" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="24.453125" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="24.726562" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="11.363281" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="19.179688" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.269531" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="15.542969" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="17" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="30.816406" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="24.453125" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="24.726562" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="13.726562" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="15.089844" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="29.816406" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <x:c r="A1" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="B1" s="5" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
+      <x:c r="C1" s="5" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="D1" s="5" t="s">
         <x:v>162</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
+      <x:c r="E1" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F1" s="5" t="s">
         <x:v>163</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+      <x:c r="G1" s="5" t="s">
         <x:v>164</x:v>
+      </x:c>
+      <x:c r="H1" s="5" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="I1" s="5" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="J1" s="5" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="K1" s="4" t="s">
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="B2" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="B3" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="B4" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="B5" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>201</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>

<commit_message>
Modified employees excel file to resolve conflict
</commit_message>
<xml_diff>
--- a/Data/Input/EmployeesInformations.xlsx
+++ b/Data/Input/EmployeesInformations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate\RPA\MetaMarian\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D59A35D-E61A-41D8-BF5A-CBE56F70292D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781690BB-AC28-4F8E-B099-CB9E402E68A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="172">
   <si>
     <t>First Name</t>
   </si>
@@ -538,6 +538,15 @@
   </si>
   <si>
     <t>Number of practical hours required</t>
+  </si>
+  <si>
+    <t>Dutu</t>
+  </si>
+  <si>
+    <t>Bucuresti</t>
+  </si>
+  <si>
+    <t>mariadutu.d@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -936,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,7 +1266,30 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D13" s="1"/>
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
@@ -1759,7 +1791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED66431-CCB8-4368-A5F8-F715BF9B41A6}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>